<commit_message>
edit and create new files for parser
</commit_message>
<xml_diff>
--- a/app/api_v1/parser/file.xlsx
+++ b/app/api_v1/parser/file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>Артикул</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Mahle---Knecht</t>
+  </si>
+  <si>
+    <t>ГАЗ</t>
+  </si>
+  <si>
+    <t>00008120T7</t>
+  </si>
+  <si>
+    <t>00006426YN</t>
   </si>
   <si>
     <t>02943N0</t>
@@ -412,7 +421,7 @@
   <dimension ref="A1:K217"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G9"/>
+      <selection activeCell="A9" sqref="A9:G217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +493,7 @@
     </row>
     <row r="3" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
@@ -493,7 +502,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -564,8 +573,8 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>82026</v>
+      <c r="A6" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
@@ -573,14 +582,14 @@
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2">
-        <v>82026</v>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
@@ -592,22 +601,22 @@
     </row>
     <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -619,22 +628,22 @@
     </row>
     <row r="8" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>362312</v>
+        <v>6270000290</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2">
-        <v>362312</v>
+        <v>6270000290</v>
       </c>
       <c r="E8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -645,27 +654,13 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1">
-        <v>2</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>

</xml_diff>